<commit_message>
Add uncertainities to average. Modify saving
</commit_message>
<xml_diff>
--- a/CR.xlsx
+++ b/CR.xlsx
@@ -523,47 +523,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>homecaillotDesktopOutput Algoperfect full testBBA15</t>
+          <t>homecaillotDesktopOutput Algoperfect full testBBA16</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3186445578231293</v>
+        <v>99.79513346289541</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3839676870748299</v>
+        <v>99.64100694689374</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>99.69663369117117</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>99.69663369117117</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>99.69663369117117</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>99.69663369117117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>